<commit_message>
implement config file in process, in progress
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hermeseuropegmbh-my.sharepoint.com/personal/johan_cabarcas_hermesworld_com/Documents/RPA/UiPath/CS-BOT_KISS_5 - FF-Briefe per Favorit ausdrucken/CS_BOT_KISS_5_FF_Briefe_ per_ Favorit_ ausdrucken/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{764EC598-B8A0-43C2-8819-4142AFD9DCA5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -84,28 +84,6 @@
     <t>System exception.</t>
   </si>
   <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -122,13 +100,151 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>kComputerUsername</t>
+  </si>
+  <si>
+    <t>CabarcasJoh</t>
+  </si>
+  <si>
+    <t>kKissUsername</t>
+  </si>
+  <si>
+    <t>svc_bot_kiss01</t>
+  </si>
+  <si>
+    <t>kEmailReportError</t>
+  </si>
+  <si>
+    <t>kApplicationUrl</t>
+  </si>
+  <si>
+    <t>https://ks-services.hlg.de/bsicrm/?dl=outline-20253&amp;i=contact-center</t>
+  </si>
+  <si>
+    <t>kFavoriteNameGroup</t>
+  </si>
+  <si>
+    <t>Freigegebene Favoriten</t>
+  </si>
+  <si>
+    <t>kPrinterName</t>
+  </si>
+  <si>
+    <t>PRT-E4-5106-09</t>
+  </si>
+  <si>
+    <t>kEmailUsername</t>
+  </si>
+  <si>
+    <t>rpa-bot01</t>
+  </si>
+  <si>
+    <t>kEmailHostName</t>
+  </si>
+  <si>
+    <t>imap01.doa.otc.hlg.de</t>
+  </si>
+  <si>
+    <t>kOutgoingEmailPort</t>
+  </si>
+  <si>
+    <t>kIncomingEmailPort</t>
+  </si>
+  <si>
+    <t>kPathFilesToPrint</t>
+  </si>
+  <si>
+    <t>kPathPrintedFiles</t>
+  </si>
+  <si>
+    <t>kPathFilesManualChk</t>
+  </si>
+  <si>
+    <t>kPathLogFolder</t>
+  </si>
+  <si>
+    <t>kPathReportFolder</t>
+  </si>
+  <si>
+    <t>kPathScreenShots</t>
+  </si>
+  <si>
+    <t>delayXXSmallms</t>
+  </si>
+  <si>
+    <t>delayXSmallms</t>
+  </si>
+  <si>
+    <t>delaySmallms</t>
+  </si>
+  <si>
+    <t>delayMediumms</t>
+  </si>
+  <si>
+    <t>delayLongms</t>
+  </si>
+  <si>
+    <t>delayXLongms</t>
+  </si>
+  <si>
+    <t>delayXSmallsec</t>
+  </si>
+  <si>
+    <t>delaySmallsec</t>
+  </si>
+  <si>
+    <t>delayMediumsec</t>
+  </si>
+  <si>
+    <t>delayLongsec</t>
+  </si>
+  <si>
+    <t>delayXlongsec</t>
+  </si>
+  <si>
+    <t>delayXXLongsec</t>
+  </si>
+  <si>
+    <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\download\\</t>
+  </si>
+  <si>
+    <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\Printed\\</t>
+  </si>
+  <si>
+    <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\ManualCheck\\</t>
+  </si>
+  <si>
+    <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\Logs\\</t>
+  </si>
+  <si>
+    <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\Reports\\</t>
+  </si>
+  <si>
+    <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\Screenshots\\</t>
+  </si>
+  <si>
+    <t>johan.cabarcas@hermesworld.com</t>
+  </si>
+  <si>
+    <t>Daten_Dokumente_Hermes</t>
+  </si>
+  <si>
+    <t>Fach 1</t>
+  </si>
+  <si>
+    <t>Daten_Dokumente_DB</t>
+  </si>
+  <si>
+    <t>Fach 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +268,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,10 +292,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -183,9 +306,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,7 +327,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,14 +625,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="104.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -546,72 +672,320 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="5">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="5">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1563,8 +1937,12 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{33130285-A137-4B6C-8759-86F3D88E52C2}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{2B05FED8-7918-45F8-9E44-11F821BF9C2D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1572,9 +1950,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -1616,85 +1996,29 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
       </c>
     </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,11 +3006,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -2702,7 +3026,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Adapt process to REF
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hermeseuropegmbh-my.sharepoint.com/personal/johan_cabarcas_hermesworld_com/Documents/RPA/UiPath/CS-BOT_KISS_5 - FF-Briefe per Favorit ausdrucken/CS_BOT_KISS_5_FF_Briefe_ per_ Favorit_ ausdrucken/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{764EC598-B8A0-43C2-8819-4142AFD9DCA5}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1C18684C-6B11-46FD-9C83-E2EF2156BBCF}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\Logs\\</t>
   </si>
   <si>
-    <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\Reports\\</t>
-  </si>
-  <si>
     <t>S:\\HG\\Allgemein\\ProcessAutomation\\DEV\\CS\\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\\Screenshots\\</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>Fach 3</t>
+  </si>
+  <si>
+    <t>S:\HG\Allgemein\ProcessAutomation\DEV\CS\BOT_KISS_5-FF-BriefePerFavoritAusdrucken\Reports\</t>
   </si>
 </sst>
 </file>
@@ -626,7 +626,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -693,7 +693,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -790,7 +790,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
@@ -798,7 +798,7 @@
         <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -1998,18 +1998,18 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
         <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>